<commit_message>
update Tx counties realtime R0 until 4/30
</commit_message>
<xml_diff>
--- a/TSHS_CaseCountData/Texas COVID-19 Case Count Data by County.xlsx
+++ b/TSHS_CaseCountData/Texas COVID-19 Case Count Data by County.xlsx
@@ -1,21 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CHS-AAU\Epi\Covid\For Ektron\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imant\Desktop\vm_share\github_project\covid-19-county-R0\TSHS_CaseCountData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AD9DE9E2-FA02-414F-B5B1-A3DDA6458D35}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C2357D-B8E2-44A1-9D79-CEDA76FD5F23}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12413" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COVID-19 Cases" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -861,10 +869,6 @@
     <t>Sabine</t>
   </si>
   <si>
-    <t>San
-Augustine</t>
-  </si>
-  <si>
     <t>San Jacinto</t>
   </si>
   <si>
@@ -1048,16 +1052,20 @@
     <t>On March 24, DSHS updated the method of reporting COVID-19 cases in Texas to provide the public with more timely information. The DSHS daily case count now includes all cases reported publicly by local health departments around the state. That change led to the report of an additional 305 cases in the March 24 total.
 The case counts do not include people who were repatriated from China or a cruise ship on U.S. government flights to JBSA-Lackland in San Antonio.</t>
   </si>
+  <si>
+    <t>San Augustine</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="###,###,###,###,##0"/>
-    <numFmt numFmtId="165" formatCode="###,##0"/>
+    <numFmt numFmtId="176" formatCode="###,###,###,###,##0"/>
+    <numFmt numFmtId="177" formatCode="###,##0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="9.5"/>
       <color rgb="FF000000"/>
@@ -1086,6 +1094,18 @@
     </font>
     <font>
       <b/>
+      <sz val="9.5"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="DengXian"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="9.5"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -1170,14 +1190,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1187,7 +1204,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1196,14 +1213,17 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1340,9 +1360,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BE267"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A195" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A206" sqref="A206"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
@@ -1350,133 +1372,133 @@
     <col min="57" max="57" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" ht="16.05" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="6"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
-      <c r="AG1" s="6"/>
-      <c r="AH1" s="6"/>
-      <c r="AI1" s="6"/>
-      <c r="AJ1" s="6"/>
-      <c r="AK1" s="6"/>
-      <c r="AL1" s="6"/>
-      <c r="AM1" s="6"/>
-      <c r="AN1" s="6"/>
-      <c r="AO1" s="6"/>
-      <c r="AP1" s="6"/>
-      <c r="AQ1" s="6"/>
-      <c r="AR1" s="6"/>
-      <c r="AS1" s="6"/>
-      <c r="AT1" s="6"/>
-      <c r="AU1" s="6"/>
-      <c r="AV1" s="6"/>
-      <c r="AW1" s="6"/>
-      <c r="AX1" s="6"/>
-      <c r="AY1" s="6"/>
-      <c r="AZ1" s="6"/>
-      <c r="BA1" s="6"/>
-      <c r="BB1" s="6"/>
-      <c r="BC1" s="6"/>
-      <c r="BD1" s="6"/>
-      <c r="BE1" s="6"/>
+    <row r="1" spans="1:57" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5"/>
+      <c r="AG1" s="5"/>
+      <c r="AH1" s="5"/>
+      <c r="AI1" s="5"/>
+      <c r="AJ1" s="5"/>
+      <c r="AK1" s="5"/>
+      <c r="AL1" s="5"/>
+      <c r="AM1" s="5"/>
+      <c r="AN1" s="5"/>
+      <c r="AO1" s="5"/>
+      <c r="AP1" s="5"/>
+      <c r="AQ1" s="5"/>
+      <c r="AR1" s="5"/>
+      <c r="AS1" s="5"/>
+      <c r="AT1" s="5"/>
+      <c r="AU1" s="5"/>
+      <c r="AV1" s="5"/>
+      <c r="AW1" s="5"/>
+      <c r="AX1" s="5"/>
+      <c r="AY1" s="5"/>
+      <c r="AZ1" s="5"/>
+      <c r="BA1" s="5"/>
+      <c r="BB1" s="5"/>
+      <c r="BC1" s="5"/>
+      <c r="BD1" s="5"/>
+      <c r="BE1" s="5"/>
     </row>
-    <row r="2" spans="1:57" ht="16.05" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6"/>
-      <c r="AB2" s="6"/>
-      <c r="AC2" s="6"/>
-      <c r="AD2" s="6"/>
-      <c r="AE2" s="6"/>
-      <c r="AF2" s="6"/>
-      <c r="AG2" s="6"/>
-      <c r="AH2" s="6"/>
-      <c r="AI2" s="6"/>
-      <c r="AJ2" s="6"/>
-      <c r="AK2" s="6"/>
-      <c r="AL2" s="6"/>
-      <c r="AM2" s="6"/>
-      <c r="AN2" s="6"/>
-      <c r="AO2" s="6"/>
-      <c r="AP2" s="6"/>
-      <c r="AQ2" s="6"/>
-      <c r="AR2" s="6"/>
-      <c r="AS2" s="6"/>
-      <c r="AT2" s="6"/>
-      <c r="AU2" s="6"/>
-      <c r="AV2" s="6"/>
-      <c r="AW2" s="6"/>
-      <c r="AX2" s="6"/>
-      <c r="AY2" s="6"/>
-      <c r="AZ2" s="6"/>
-      <c r="BA2" s="6"/>
-      <c r="BB2" s="6"/>
-      <c r="BC2" s="6"/>
-      <c r="BD2" s="6"/>
-      <c r="BE2" s="6"/>
+    <row r="2" spans="1:57" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
+      <c r="AG2" s="5"/>
+      <c r="AH2" s="5"/>
+      <c r="AI2" s="5"/>
+      <c r="AJ2" s="5"/>
+      <c r="AK2" s="5"/>
+      <c r="AL2" s="5"/>
+      <c r="AM2" s="5"/>
+      <c r="AN2" s="5"/>
+      <c r="AO2" s="5"/>
+      <c r="AP2" s="5"/>
+      <c r="AQ2" s="5"/>
+      <c r="AR2" s="5"/>
+      <c r="AS2" s="5"/>
+      <c r="AT2" s="5"/>
+      <c r="AU2" s="5"/>
+      <c r="AV2" s="5"/>
+      <c r="AW2" s="5"/>
+      <c r="AX2" s="5"/>
+      <c r="AY2" s="5"/>
+      <c r="AZ2" s="5"/>
+      <c r="BA2" s="5"/>
+      <c r="BB2" s="5"/>
+      <c r="BC2" s="5"/>
+      <c r="BD2" s="5"/>
+      <c r="BE2" s="5"/>
     </row>
-    <row r="3" spans="1:57" ht="36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:57" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1645,7 +1667,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>59</v>
       </c>
@@ -1818,7 +1840,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>60</v>
       </c>
@@ -1991,7 +2013,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>61</v>
       </c>
@@ -2164,7 +2186,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>62</v>
       </c>
@@ -2337,7 +2359,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>63</v>
       </c>
@@ -2510,7 +2532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>64</v>
       </c>
@@ -2683,7 +2705,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>65</v>
       </c>
@@ -2856,7 +2878,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>66</v>
       </c>
@@ -3029,7 +3051,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>67</v>
       </c>
@@ -3202,7 +3224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>68</v>
       </c>
@@ -3375,7 +3397,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>69</v>
       </c>
@@ -3548,7 +3570,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>70</v>
       </c>
@@ -3721,7 +3743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>71</v>
       </c>
@@ -3894,7 +3916,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>72</v>
       </c>
@@ -4067,7 +4089,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="18" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>73</v>
       </c>
@@ -4240,7 +4262,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="19" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>74</v>
       </c>
@@ -4413,7 +4435,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>75</v>
       </c>
@@ -4586,7 +4608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>76</v>
       </c>
@@ -4759,7 +4781,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>77</v>
       </c>
@@ -4932,7 +4954,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>78</v>
       </c>
@@ -5105,7 +5127,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="24" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>79</v>
       </c>
@@ -5278,7 +5300,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="25" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>80</v>
       </c>
@@ -5451,7 +5473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>81</v>
       </c>
@@ -5624,7 +5646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>82</v>
       </c>
@@ -5797,7 +5819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>83</v>
       </c>
@@ -5970,7 +5992,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>84</v>
       </c>
@@ -6143,7 +6165,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>85</v>
       </c>
@@ -6316,7 +6338,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>86</v>
       </c>
@@ -6489,7 +6511,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>87</v>
       </c>
@@ -6662,7 +6684,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>88</v>
       </c>
@@ -6835,7 +6857,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>89</v>
       </c>
@@ -7008,7 +7030,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="35" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>90</v>
       </c>
@@ -7181,7 +7203,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>91</v>
       </c>
@@ -7354,7 +7376,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>92</v>
       </c>
@@ -7527,7 +7549,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>93</v>
       </c>
@@ -7700,7 +7722,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>94</v>
       </c>
@@ -7873,7 +7895,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>95</v>
       </c>
@@ -8046,7 +8068,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>96</v>
       </c>
@@ -8219,7 +8241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>97</v>
       </c>
@@ -8392,7 +8414,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>98</v>
       </c>
@@ -8565,7 +8587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>99</v>
       </c>
@@ -8738,7 +8760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>100</v>
       </c>
@@ -8911,7 +8933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>101</v>
       </c>
@@ -9084,7 +9106,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="47" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>102</v>
       </c>
@@ -9257,7 +9279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>103</v>
       </c>
@@ -9430,7 +9452,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>104</v>
       </c>
@@ -9603,7 +9625,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>105</v>
       </c>
@@ -9776,7 +9798,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>106</v>
       </c>
@@ -9949,7 +9971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>107</v>
       </c>
@@ -10122,7 +10144,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>108</v>
       </c>
@@ -10295,7 +10317,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="54" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>109</v>
       </c>
@@ -10468,7 +10490,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>110</v>
       </c>
@@ -10641,7 +10663,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>111</v>
       </c>
@@ -10814,7 +10836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>112</v>
       </c>
@@ -10987,7 +11009,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>113</v>
       </c>
@@ -11160,7 +11182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>114</v>
       </c>
@@ -11333,7 +11355,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>115</v>
       </c>
@@ -11506,7 +11528,7 @@
         <v>3352</v>
       </c>
     </row>
-    <row r="61" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>116</v>
       </c>
@@ -11679,7 +11701,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="62" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>117</v>
       </c>
@@ -11852,7 +11874,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="63" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>118</v>
       </c>
@@ -12025,7 +12047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>119</v>
       </c>
@@ -12198,7 +12220,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="65" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>120</v>
       </c>
@@ -12371,7 +12393,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>121</v>
       </c>
@@ -12544,7 +12566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>122</v>
       </c>
@@ -12717,7 +12739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>123</v>
       </c>
@@ -12890,7 +12912,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="69" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>124</v>
       </c>
@@ -13063,7 +13085,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>125</v>
       </c>
@@ -13236,7 +13258,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>126</v>
       </c>
@@ -13409,7 +13431,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="72" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>127</v>
       </c>
@@ -13582,7 +13604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>128</v>
       </c>
@@ -13755,7 +13777,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="74" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>129</v>
       </c>
@@ -13928,7 +13950,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="75" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>130</v>
       </c>
@@ -14101,7 +14123,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="76" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>131</v>
       </c>
@@ -14274,7 +14296,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>132</v>
       </c>
@@ -14447,7 +14469,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>133</v>
       </c>
@@ -14620,7 +14642,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="79" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>134</v>
       </c>
@@ -14793,7 +14815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>135</v>
       </c>
@@ -14966,7 +14988,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>136</v>
       </c>
@@ -15139,7 +15161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>137</v>
       </c>
@@ -15312,7 +15334,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="83" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>138</v>
       </c>
@@ -15485,7 +15507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>139</v>
       </c>
@@ -15658,7 +15680,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>140</v>
       </c>
@@ -15831,7 +15853,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>141</v>
       </c>
@@ -16004,7 +16026,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>142</v>
       </c>
@@ -16177,7 +16199,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="88" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>143</v>
       </c>
@@ -16350,7 +16372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>144</v>
       </c>
@@ -16523,7 +16545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>145</v>
       </c>
@@ -16696,7 +16718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>146</v>
       </c>
@@ -16869,7 +16891,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>147</v>
       </c>
@@ -17042,7 +17064,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="93" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>148</v>
       </c>
@@ -17215,7 +17237,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="94" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>149</v>
       </c>
@@ -17388,7 +17410,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="95" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>150</v>
       </c>
@@ -17561,7 +17583,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="96" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>151</v>
       </c>
@@ -17734,7 +17756,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="97" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>152</v>
       </c>
@@ -17907,7 +17929,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="98" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>153</v>
       </c>
@@ -18080,7 +18102,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="99" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>154</v>
       </c>
@@ -18253,7 +18275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>155</v>
       </c>
@@ -18426,7 +18448,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>156</v>
       </c>
@@ -18599,7 +18621,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="102" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>157</v>
       </c>
@@ -18772,7 +18794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>158</v>
       </c>
@@ -18945,7 +18967,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="104" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>159</v>
       </c>
@@ -19118,7 +19140,7 @@
         <v>6161</v>
       </c>
     </row>
-    <row r="105" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>160</v>
       </c>
@@ -19291,7 +19313,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="106" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>161</v>
       </c>
@@ -19464,7 +19486,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>162</v>
       </c>
@@ -19637,7 +19659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>163</v>
       </c>
@@ -19810,7 +19832,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="109" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>164</v>
       </c>
@@ -19983,7 +20005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>165</v>
       </c>
@@ -20156,7 +20178,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="111" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>166</v>
       </c>
@@ -20329,7 +20351,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="112" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>167</v>
       </c>
@@ -20502,7 +20524,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="113" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>168</v>
       </c>
@@ -20675,7 +20697,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="114" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>169</v>
       </c>
@@ -20848,7 +20870,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="115" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>170</v>
       </c>
@@ -21021,7 +21043,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>171</v>
       </c>
@@ -21194,7 +21216,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>172</v>
       </c>
@@ -21367,7 +21389,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>173</v>
       </c>
@@ -21540,7 +21562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>174</v>
       </c>
@@ -21713,7 +21735,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="120" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>175</v>
       </c>
@@ -21886,7 +21908,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="121" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>176</v>
       </c>
@@ -22059,7 +22081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>177</v>
       </c>
@@ -22232,7 +22254,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="123" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
         <v>178</v>
       </c>
@@ -22405,7 +22427,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="124" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>179</v>
       </c>
@@ -22578,7 +22600,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="125" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>180</v>
       </c>
@@ -22751,7 +22773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>181</v>
       </c>
@@ -22924,7 +22946,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="127" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>182</v>
       </c>
@@ -23097,7 +23119,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="128" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>183</v>
       </c>
@@ -23270,7 +23292,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="129" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>184</v>
       </c>
@@ -23443,7 +23465,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="130" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
         <v>185</v>
       </c>
@@ -23616,7 +23638,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="131" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>186</v>
       </c>
@@ -23789,7 +23811,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="132" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>187</v>
       </c>
@@ -23962,7 +23984,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="133" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>188</v>
       </c>
@@ -24135,7 +24157,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="134" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>189</v>
       </c>
@@ -24308,7 +24330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>190</v>
       </c>
@@ -24481,7 +24503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
         <v>191</v>
       </c>
@@ -24654,7 +24676,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="137" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>192</v>
       </c>
@@ -24827,7 +24849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
         <v>193</v>
       </c>
@@ -25000,7 +25022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>194</v>
       </c>
@@ -25173,7 +25195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
         <v>195</v>
       </c>
@@ -25346,7 +25368,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="141" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
         <v>196</v>
       </c>
@@ -25519,7 +25541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
         <v>197</v>
       </c>
@@ -25692,7 +25714,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="143" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>198</v>
       </c>
@@ -25865,7 +25887,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="144" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
         <v>199</v>
       </c>
@@ -26038,7 +26060,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="145" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
         <v>200</v>
       </c>
@@ -26211,7 +26233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
         <v>201</v>
       </c>
@@ -26384,7 +26406,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="147" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>202</v>
       </c>
@@ -26557,7 +26579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="148" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
         <v>203</v>
       </c>
@@ -26730,7 +26752,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="149" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
         <v>204</v>
       </c>
@@ -26903,7 +26925,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="150" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
         <v>205</v>
       </c>
@@ -27076,7 +27098,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="151" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
         <v>206</v>
       </c>
@@ -27249,7 +27271,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="152" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
         <v>207</v>
       </c>
@@ -27422,7 +27444,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="153" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
         <v>208</v>
       </c>
@@ -27595,7 +27617,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="154" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
         <v>209</v>
       </c>
@@ -27768,7 +27790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
         <v>210</v>
       </c>
@@ -27941,7 +27963,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="156" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
         <v>211</v>
       </c>
@@ -28114,7 +28136,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="157" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
         <v>212</v>
       </c>
@@ -28287,7 +28309,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="158" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
         <v>213</v>
       </c>
@@ -28460,7 +28482,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="159" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
         <v>214</v>
       </c>
@@ -28633,7 +28655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
         <v>215</v>
       </c>
@@ -28806,7 +28828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
         <v>216</v>
       </c>
@@ -28979,7 +29001,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="162" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
         <v>217</v>
       </c>
@@ -29152,7 +29174,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="163" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
         <v>218</v>
       </c>
@@ -29325,7 +29347,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="164" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
         <v>219</v>
       </c>
@@ -29498,7 +29520,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="165" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
         <v>220</v>
       </c>
@@ -29671,7 +29693,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="166" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
         <v>221</v>
       </c>
@@ -29844,7 +29866,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="167" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
         <v>222</v>
       </c>
@@ -30017,7 +30039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
         <v>223</v>
       </c>
@@ -30190,7 +30212,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="169" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
         <v>224</v>
       </c>
@@ -30363,7 +30385,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="170" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
         <v>225</v>
       </c>
@@ -30536,7 +30558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
         <v>226</v>
       </c>
@@ -30709,7 +30731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="2" t="s">
         <v>227</v>
       </c>
@@ -30882,7 +30904,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="173" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
         <v>228</v>
       </c>
@@ -31055,7 +31077,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="174" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
         <v>229</v>
       </c>
@@ -31228,7 +31250,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="175" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
         <v>230</v>
       </c>
@@ -31401,7 +31423,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="176" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="2" t="s">
         <v>231</v>
       </c>
@@ -31574,7 +31596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="2" t="s">
         <v>232</v>
       </c>
@@ -31747,7 +31769,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="178" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="2" t="s">
         <v>233</v>
       </c>
@@ -31920,7 +31942,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="179" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="2" t="s">
         <v>234</v>
       </c>
@@ -32093,7 +32115,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="180" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="2" t="s">
         <v>235</v>
       </c>
@@ -32266,7 +32288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="2" t="s">
         <v>236</v>
       </c>
@@ -32439,7 +32461,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="182" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="2" t="s">
         <v>237</v>
       </c>
@@ -32612,7 +32634,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="183" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="2" t="s">
         <v>238</v>
       </c>
@@ -32785,7 +32807,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="184" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="2" t="s">
         <v>239</v>
       </c>
@@ -32958,7 +32980,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="185" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="2" t="s">
         <v>240</v>
       </c>
@@ -33131,7 +33153,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="186" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="2" t="s">
         <v>241</v>
       </c>
@@ -33304,7 +33326,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="187" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="2" t="s">
         <v>242</v>
       </c>
@@ -33477,7 +33499,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="188" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="2" t="s">
         <v>243</v>
       </c>
@@ -33650,7 +33672,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="189" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="2" t="s">
         <v>244</v>
       </c>
@@ -33823,7 +33845,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="190" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="2" t="s">
         <v>245</v>
       </c>
@@ -33996,7 +34018,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="191" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="2" t="s">
         <v>246</v>
       </c>
@@ -34169,7 +34191,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="192" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="2" t="s">
         <v>247</v>
       </c>
@@ -34342,7 +34364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="2" t="s">
         <v>248</v>
       </c>
@@ -34515,7 +34537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="194" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="2" t="s">
         <v>249</v>
       </c>
@@ -34688,7 +34710,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="195" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="2" t="s">
         <v>250</v>
       </c>
@@ -34861,7 +34883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="2" t="s">
         <v>251</v>
       </c>
@@ -35034,7 +35056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="2" t="s">
         <v>252</v>
       </c>
@@ -35207,7 +35229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="2" t="s">
         <v>253</v>
       </c>
@@ -35380,7 +35402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="2" t="s">
         <v>254</v>
       </c>
@@ -35553,7 +35575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="2" t="s">
         <v>255</v>
       </c>
@@ -35726,7 +35748,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="201" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="2" t="s">
         <v>256</v>
       </c>
@@ -35899,7 +35921,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="202" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="2" t="s">
         <v>257</v>
       </c>
@@ -36072,7 +36094,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="203" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="2" t="s">
         <v>258</v>
       </c>
@@ -36245,7 +36267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="2" t="s">
         <v>259</v>
       </c>
@@ -36418,7 +36440,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="205" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="2" t="s">
         <v>260</v>
       </c>
@@ -36591,9 +36613,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:57" ht="29" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A206" s="5" t="s">
-        <v>261</v>
+    <row r="206" spans="1:57" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A206" s="15" t="s">
+        <v>321</v>
       </c>
       <c r="B206" s="3">
         <v>9340</v>
@@ -36764,9 +36786,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="207" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B207" s="3">
         <v>32428</v>
@@ -36937,9 +36959,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="208" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B208" s="3">
         <v>68331</v>
@@ -37110,9 +37132,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="209" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B209" s="3">
         <v>6482</v>
@@ -37283,9 +37305,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B210" s="3">
         <v>3920</v>
@@ -37456,9 +37478,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B211" s="3">
         <v>18906</v>
@@ -37629,9 +37651,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="212" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B212" s="3">
         <v>3734</v>
@@ -37802,9 +37824,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B213" s="3">
         <v>28649</v>
@@ -37975,9 +37997,9 @@
         <v>106</v>
       </c>
     </row>
-    <row r="214" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B214" s="3">
         <v>3440</v>
@@ -38148,9 +38170,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="215" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B215" s="3">
         <v>243064</v>
@@ -38321,9 +38343,9 @@
         <v>142</v>
       </c>
     </row>
-    <row r="216" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B216" s="3">
         <v>10480</v>
@@ -38494,9 +38516,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B217" s="3">
         <v>68878</v>
@@ -38667,9 +38689,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="218" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B218" s="3">
         <v>10297</v>
@@ -38840,9 +38862,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A219" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B219" s="3">
         <v>1214</v>
@@ -39013,9 +39035,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B220" s="3">
         <v>1515</v>
@@ -39186,9 +39208,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B221" s="3">
         <v>4651</v>
@@ -39359,9 +39381,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B222" s="3">
         <v>8230</v>
@@ -39532,9 +39554,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="223" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B223" s="3">
         <v>2127850</v>
@@ -39705,9 +39727,9 @@
         <v>2149</v>
       </c>
     </row>
-    <row r="224" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A224" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B224" s="3">
         <v>138279</v>
@@ -39878,9 +39900,9 @@
         <v>291</v>
       </c>
     </row>
-    <row r="225" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B225" s="3">
         <v>1047</v>
@@ -40051,9 +40073,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A226" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B226" s="3">
         <v>13323</v>
@@ -40224,9 +40246,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="227" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A227" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B227" s="3">
         <v>1639</v>
@@ -40397,9 +40419,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A228" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B228" s="3">
         <v>37790</v>
@@ -40570,9 +40592,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="229" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A229" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B229" s="3">
         <v>114995</v>
@@ -40743,9 +40765,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="230" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A230" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B230" s="3">
         <v>1277007</v>
@@ -40916,9 +40938,9 @@
         <v>1591</v>
       </c>
     </row>
-    <row r="231" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A231" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B231" s="3">
         <v>16618</v>
@@ -41089,9 +41111,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="232" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A232" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B232" s="3">
         <v>22646</v>
@@ -41262,9 +41284,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="233" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A233" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B233" s="3">
         <v>45120</v>
@@ -41435,9 +41457,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="234" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A234" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B234" s="3">
         <v>3886</v>
@@ -41608,9 +41630,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A235" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B235" s="3">
         <v>28593</v>
@@ -41781,9 +41803,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="236" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A236" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B236" s="3">
         <v>53256</v>
@@ -41954,9 +41976,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="237" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A237" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B237" s="3">
         <v>58259</v>
@@ -42127,9 +42149,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="238" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A238" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B238" s="3">
         <v>92845</v>
@@ -42300,9 +42322,9 @@
         <v>132</v>
       </c>
     </row>
-    <row r="239" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A239" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B239" s="3">
         <v>72778</v>
@@ -42473,9 +42495,9 @@
         <v>245</v>
       </c>
     </row>
-    <row r="240" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A240" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B240" s="3">
         <v>58002</v>
@@ -42646,9 +42668,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="241" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A241" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B241" s="3">
         <v>11213</v>
@@ -42819,9 +42841,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A242" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B242" s="3">
         <v>37673</v>
@@ -42992,9 +43014,9 @@
         <v>142</v>
       </c>
     </row>
-    <row r="243" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A243" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B243" s="3">
         <v>317733</v>
@@ -43165,9 +43187,9 @@
         <v>358</v>
       </c>
     </row>
-    <row r="244" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A244" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B244" s="3">
         <v>43271</v>
@@ -43338,9 +43360,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="245" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A245" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B245" s="3">
         <v>5934</v>
@@ -43511,9 +43533,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="246" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A246" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B246" s="3">
         <v>133363</v>
@@ -43684,9 +43706,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="247" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A247" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B247" s="3">
         <v>14897</v>
@@ -43857,9 +43879,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A248" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B248" s="3">
         <v>26817</v>
@@ -44030,9 +44052,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="249" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A249" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B249" s="3">
         <v>633783</v>
@@ -44203,9 +44225,9 @@
         <v>293</v>
       </c>
     </row>
-    <row r="250" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A250" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B250" s="3">
         <v>57292</v>
@@ -44376,9 +44398,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="251" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A251" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B251" s="3">
         <v>8371</v>
@@ -44549,9 +44571,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="252" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A252" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B252" s="3">
         <v>74490</v>
@@ -44722,9 +44744,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="253" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A253" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B253" s="3">
         <v>48594</v>
@@ -44895,9 +44917,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="254" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A254" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B254" s="3">
         <v>9591</v>
@@ -45068,9 +45090,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A255" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B255" s="3">
         <v>19914</v>
@@ -45241,9 +45263,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="256" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A256" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B256" s="3">
         <v>17043</v>
@@ -45414,9 +45436,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="257" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A257" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B257" s="3">
         <v>12895</v>
@@ -45587,180 +45609,180 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:57" s="15" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A258" s="12" t="s">
-        <v>313</v>
-      </c>
-      <c r="B258" s="13">
+    <row r="258" spans="1:57" s="14" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A258" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="B258" s="12">
         <v>30541978</v>
       </c>
-      <c r="C258" s="13">
-        <v>0</v>
-      </c>
-      <c r="D258" s="13">
-        <v>0</v>
-      </c>
-      <c r="E258" s="13">
+      <c r="C258" s="12">
+        <v>0</v>
+      </c>
+      <c r="D258" s="12">
+        <v>0</v>
+      </c>
+      <c r="E258" s="12">
         <v>5</v>
       </c>
-      <c r="F258" s="13">
+      <c r="F258" s="12">
         <v>12</v>
       </c>
-      <c r="G258" s="13">
+      <c r="G258" s="12">
         <v>15</v>
       </c>
-      <c r="H258" s="13">
+      <c r="H258" s="12">
         <v>18</v>
       </c>
-      <c r="I258" s="13">
+      <c r="I258" s="12">
         <v>22</v>
       </c>
-      <c r="J258" s="13">
+      <c r="J258" s="12">
         <v>22</v>
       </c>
-      <c r="K258" s="13">
+      <c r="K258" s="12">
         <v>56</v>
       </c>
-      <c r="L258" s="13">
+      <c r="L258" s="12">
         <v>56</v>
       </c>
-      <c r="M258" s="13">
+      <c r="M258" s="12">
         <v>63</v>
       </c>
-      <c r="N258" s="13">
+      <c r="N258" s="12">
         <v>82</v>
       </c>
-      <c r="O258" s="13">
+      <c r="O258" s="12">
         <v>108</v>
       </c>
-      <c r="P258" s="13">
+      <c r="P258" s="12">
         <v>175</v>
       </c>
-      <c r="Q258" s="13">
+      <c r="Q258" s="12">
         <v>235</v>
       </c>
-      <c r="R258" s="13">
+      <c r="R258" s="12">
         <v>263</v>
       </c>
-      <c r="S258" s="13">
+      <c r="S258" s="12">
         <v>287</v>
       </c>
-      <c r="T258" s="13">
+      <c r="T258" s="12">
         <v>712</v>
       </c>
-      <c r="U258" s="13">
+      <c r="U258" s="12">
         <v>975</v>
       </c>
-      <c r="V258" s="13">
+      <c r="V258" s="12">
         <v>1394</v>
       </c>
-      <c r="W258" s="13">
+      <c r="W258" s="12">
         <v>1731</v>
       </c>
-      <c r="X258" s="13">
+      <c r="X258" s="12">
         <v>2048</v>
       </c>
-      <c r="Y258" s="13">
+      <c r="Y258" s="12">
         <v>2552</v>
       </c>
-      <c r="Z258" s="13">
+      <c r="Z258" s="12">
         <v>2874</v>
       </c>
-      <c r="AA258" s="13">
+      <c r="AA258" s="12">
         <v>3266</v>
       </c>
-      <c r="AB258" s="13">
+      <c r="AB258" s="12">
         <v>3996</v>
       </c>
-      <c r="AC258" s="13">
+      <c r="AC258" s="12">
         <v>4665</v>
       </c>
-      <c r="AD258" s="13">
+      <c r="AD258" s="12">
         <v>5324</v>
       </c>
-      <c r="AE258" s="13">
+      <c r="AE258" s="12">
         <v>6112</v>
       </c>
-      <c r="AF258" s="13">
+      <c r="AF258" s="12">
         <v>6793</v>
       </c>
-      <c r="AG258" s="13">
+      <c r="AG258" s="12">
         <v>7273</v>
       </c>
-      <c r="AH258" s="13">
+      <c r="AH258" s="12">
         <v>8261</v>
       </c>
-      <c r="AI258" s="13">
+      <c r="AI258" s="12">
         <v>9353</v>
       </c>
-      <c r="AJ258" s="13">
+      <c r="AJ258" s="12">
         <v>10230</v>
       </c>
-      <c r="AK258" s="13">
+      <c r="AK258" s="12">
         <v>11671</v>
       </c>
-      <c r="AL258" s="13">
+      <c r="AL258" s="12">
         <v>12561</v>
       </c>
-      <c r="AM258" s="13">
+      <c r="AM258" s="12">
         <v>13484</v>
       </c>
-      <c r="AN258" s="13">
+      <c r="AN258" s="12">
         <v>13906</v>
       </c>
-      <c r="AO258" s="13">
+      <c r="AO258" s="12">
         <v>14624</v>
       </c>
-      <c r="AP258" s="13">
+      <c r="AP258" s="12">
         <v>15492</v>
       </c>
-      <c r="AQ258" s="13">
+      <c r="AQ258" s="12">
         <v>16455</v>
       </c>
-      <c r="AR258" s="13">
+      <c r="AR258" s="12">
         <v>17371</v>
       </c>
-      <c r="AS258" s="13">
+      <c r="AS258" s="12">
         <v>18260</v>
       </c>
-      <c r="AT258" s="13">
+      <c r="AT258" s="12">
         <v>18923</v>
       </c>
-      <c r="AU258" s="13">
+      <c r="AU258" s="12">
         <v>19458</v>
       </c>
-      <c r="AV258" s="13">
+      <c r="AV258" s="12">
         <v>20196</v>
       </c>
-      <c r="AW258" s="13">
+      <c r="AW258" s="12">
         <v>21069</v>
       </c>
-      <c r="AX258" s="13">
+      <c r="AX258" s="12">
         <v>21944</v>
       </c>
-      <c r="AY258" s="13">
+      <c r="AY258" s="12">
         <v>22806</v>
       </c>
-      <c r="AZ258" s="13">
+      <c r="AZ258" s="12">
         <v>23773</v>
       </c>
-      <c r="BA258" s="13">
+      <c r="BA258" s="12">
         <v>24631</v>
       </c>
-      <c r="BB258" s="13">
+      <c r="BB258" s="12">
         <v>25297</v>
       </c>
-      <c r="BC258" s="13">
+      <c r="BC258" s="12">
         <v>26171</v>
       </c>
-      <c r="BD258" s="13">
+      <c r="BD258" s="12">
         <v>27054</v>
       </c>
-      <c r="BE258" s="14">
+      <c r="BE258" s="13">
         <v>28087</v>
       </c>
     </row>
-    <row r="259" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:57" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A259" s="2"/>
       <c r="B259" s="3"/>
       <c r="C259" s="3"/>
@@ -45819,212 +45841,213 @@
       <c r="BD259" s="3"/>
       <c r="BE259" s="4"/>
     </row>
-    <row r="260" spans="1:57" s="11" customFormat="1" ht="58.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A260" s="9" t="s">
-        <v>315</v>
-      </c>
-      <c r="B260" s="10" t="s">
+    <row r="260" spans="1:57" s="10" customFormat="1" ht="58.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A260" s="8" t="s">
         <v>314</v>
       </c>
-      <c r="C260" s="10">
-        <v>0</v>
-      </c>
-      <c r="D260" s="10">
-        <v>0</v>
-      </c>
-      <c r="E260" s="10">
-        <v>2</v>
-      </c>
-      <c r="F260" s="10">
-        <v>3</v>
-      </c>
-      <c r="G260" s="10">
+      <c r="B260" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="C260" s="9">
+        <v>0</v>
+      </c>
+      <c r="D260" s="9">
+        <v>0</v>
+      </c>
+      <c r="E260" s="9">
+        <v>2</v>
+      </c>
+      <c r="F260" s="9">
+        <v>3</v>
+      </c>
+      <c r="G260" s="9">
         <v>4</v>
       </c>
-      <c r="H260" s="10">
+      <c r="H260" s="9">
         <v>6</v>
       </c>
-      <c r="I260" s="10">
+      <c r="I260" s="9">
         <v>7</v>
       </c>
-      <c r="J260" s="10">
+      <c r="J260" s="9">
         <v>7</v>
       </c>
-      <c r="K260" s="10">
+      <c r="K260" s="9">
         <v>17</v>
       </c>
-      <c r="L260" s="10">
+      <c r="L260" s="9">
         <v>17</v>
       </c>
-      <c r="M260" s="10">
+      <c r="M260" s="9">
         <v>20</v>
       </c>
-      <c r="N260" s="10">
+      <c r="N260" s="9">
         <v>23</v>
       </c>
-      <c r="O260" s="10">
+      <c r="O260" s="9">
         <v>27</v>
       </c>
-      <c r="P260" s="10">
+      <c r="P260" s="9">
         <v>34</v>
       </c>
-      <c r="Q260" s="10">
+      <c r="Q260" s="9">
         <v>41</v>
       </c>
-      <c r="R260" s="10">
+      <c r="R260" s="9">
         <v>43</v>
       </c>
-      <c r="S260" s="10">
+      <c r="S260" s="9">
         <v>46</v>
       </c>
-      <c r="T260" s="10">
+      <c r="T260" s="9">
         <v>65</v>
       </c>
-      <c r="U260" s="10">
+      <c r="U260" s="9">
         <v>82</v>
       </c>
-      <c r="V260" s="10">
+      <c r="V260" s="9">
         <v>92</v>
       </c>
-      <c r="W260" s="10">
+      <c r="W260" s="9">
         <v>104</v>
       </c>
-      <c r="X260" s="10">
+      <c r="X260" s="9">
         <v>110</v>
       </c>
-      <c r="Y260" s="10">
+      <c r="Y260" s="9">
         <v>118</v>
       </c>
-      <c r="Z260" s="10">
+      <c r="Z260" s="9">
         <v>122</v>
       </c>
-      <c r="AA260" s="10">
+      <c r="AA260" s="9">
         <v>122</v>
       </c>
-      <c r="AB260" s="10">
+      <c r="AB260" s="9">
         <v>135</v>
       </c>
-      <c r="AC260" s="10">
+      <c r="AC260" s="9">
         <v>143</v>
       </c>
-      <c r="AD260" s="10">
+      <c r="AD260" s="9">
         <v>145</v>
       </c>
-      <c r="AE260" s="10">
+      <c r="AE260" s="9">
         <v>151</v>
       </c>
-      <c r="AF260" s="10">
+      <c r="AF260" s="9">
         <v>152</v>
       </c>
-      <c r="AG260" s="10">
+      <c r="AG260" s="9">
         <v>156</v>
       </c>
-      <c r="AH260" s="10">
+      <c r="AH260" s="9">
         <v>161</v>
       </c>
-      <c r="AI260" s="10">
+      <c r="AI260" s="9">
         <v>167</v>
       </c>
-      <c r="AJ260" s="10">
+      <c r="AJ260" s="9">
         <v>170</v>
       </c>
-      <c r="AK260" s="10">
+      <c r="AK260" s="9">
         <v>176</v>
       </c>
-      <c r="AL260" s="10">
+      <c r="AL260" s="9">
         <v>177</v>
       </c>
-      <c r="AM260" s="10">
+      <c r="AM260" s="9">
         <v>177</v>
       </c>
-      <c r="AN260" s="10">
+      <c r="AN260" s="9">
         <v>178</v>
       </c>
-      <c r="AO260" s="10">
+      <c r="AO260" s="9">
         <v>181</v>
       </c>
-      <c r="AP260" s="10">
+      <c r="AP260" s="9">
         <v>184</v>
       </c>
-      <c r="AQ260" s="10">
+      <c r="AQ260" s="9">
         <v>191</v>
       </c>
-      <c r="AR260" s="10">
+      <c r="AR260" s="9">
         <v>192</v>
       </c>
-      <c r="AS260" s="10">
+      <c r="AS260" s="9">
         <v>194</v>
       </c>
-      <c r="AT260" s="10">
+      <c r="AT260" s="9">
         <v>197</v>
       </c>
-      <c r="AU260" s="10">
+      <c r="AU260" s="9">
         <v>198</v>
       </c>
-      <c r="AV260" s="10">
+      <c r="AV260" s="9">
         <v>198</v>
       </c>
-      <c r="AW260" s="10">
+      <c r="AW260" s="9">
         <v>200</v>
       </c>
-      <c r="AX260" s="10">
+      <c r="AX260" s="9">
         <v>202</v>
       </c>
-      <c r="AY260" s="10">
+      <c r="AY260" s="9">
         <v>204</v>
       </c>
-      <c r="AZ260" s="10">
+      <c r="AZ260" s="9">
         <v>204</v>
       </c>
-      <c r="BA260" s="10">
+      <c r="BA260" s="9">
         <v>204</v>
       </c>
-      <c r="BB260" s="10">
+      <c r="BB260" s="9">
         <v>205</v>
       </c>
-      <c r="BC260" s="10">
+      <c r="BC260" s="9">
         <v>207</v>
       </c>
-      <c r="BD260" s="10">
+      <c r="BD260" s="9">
         <v>207</v>
       </c>
-      <c r="BE260" s="10">
+      <c r="BE260" s="9">
         <f t="shared" ref="BE260" si="0">COUNTIF(BE4:BE257,"&lt;&gt;0")</f>
         <v>209</v>
       </c>
     </row>
-    <row r="262" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="263" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A263" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="263" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A263" t="s">
+    <row r="264" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A264" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="264" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A264" t="s">
+    <row r="265" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A265" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="265" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A265" t="s">
+    <row r="266" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A266" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="266" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A266" t="s">
+    <row r="267" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A267" t="s">
         <v>320</v>
-      </c>
-    </row>
-    <row r="267" spans="1:57" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A267" t="s">
-        <v>321</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.05" right="0.05" top="0.5" bottom="0.5" header="0" footer="0"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>